<commit_message>
started SR development - práctica SR
</commit_message>
<xml_diff>
--- a/A13/Recomendación de películas mediante factorización de matrices/primera parte/primera_parte.xlsx
+++ b/A13/Recomendación de películas mediante factorización de matrices/primera parte/primera_parte.xlsx
@@ -482,1366 +482,1366 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Star Wars: Episode IV - A New Hope (1977)</t>
+          <t>Lord of the Rings: The Fellowship of the Ring, The (2001)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.01799161099940515</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.439267</v>
+        <v>-0.225569</v>
       </c>
       <c r="E2" t="n">
-        <v>-1.200818</v>
+        <v>0.240604</v>
       </c>
       <c r="F2" t="n">
-        <v>0.382361</v>
+        <v>-0.167136</v>
       </c>
       <c r="G2" t="n">
-        <v>0.199633</v>
+        <v>-1.50213</v>
       </c>
       <c r="H2" t="n">
-        <v>1.058424</v>
+        <v>1.063062</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.422181</v>
+        <v>0.389827</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>96</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Finding Nemo (2003)</t>
+          <t>Incredibles, The (2004)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.003446375623112991</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>0.288385</v>
+        <v>0.49024</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.351151</v>
+        <v>-0.924104</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.108478</v>
+        <v>0.69907</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.940476</v>
+        <v>-1.499481</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.412718</v>
+        <v>-0.09470099999999999</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.808264</v>
+        <v>-1.02732</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Forrest Gump (1994)</t>
+          <t>Schindler's List (1993)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-1.85397131883922e-05</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>0.901322</v>
+        <v>0.469902</v>
       </c>
       <c r="E4" t="n">
-        <v>0.865292</v>
+        <v>-0.059721</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.037117</v>
+        <v>0.172039</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.026354</v>
+        <v>-1.389097</v>
       </c>
       <c r="H4" t="n">
-        <v>0.988768</v>
+        <v>0.56819</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.024578</v>
+        <v>-0.008004000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>American Beauty (1999)</t>
+          <t>Bourne Supremacy, The (2004)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4.825320290461774e-05</v>
+        <v>7</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.04848</v>
+        <v>0.212682</v>
       </c>
       <c r="E5" t="n">
-        <v>0.126738</v>
+        <v>0.284779</v>
       </c>
       <c r="F5" t="n">
-        <v>0.46106</v>
+        <v>-0.921839</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.10675</v>
+        <v>-1.301435</v>
       </c>
       <c r="H5" t="n">
-        <v>0.39937</v>
+        <v>0.223149</v>
       </c>
       <c r="I5" t="n">
-        <v>0.399536</v>
+        <v>-0.150782</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pirates of the Caribbean: The Curse of the Black Pearl (2003)</t>
+          <t>Lord of the Rings: The Two Towers, The (2002)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.001133185363849456</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
-        <v>0.192967</v>
+        <v>-0.394141</v>
       </c>
       <c r="E6" t="n">
-        <v>0.262919</v>
+        <v>0.146831</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.116306</v>
+        <v>-0.410531</v>
       </c>
       <c r="G6" t="n">
-        <v>0.322482</v>
+        <v>-1.186645</v>
       </c>
       <c r="H6" t="n">
-        <v>0.723021</v>
+        <v>1.096657</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.82364</v>
+        <v>0.377764</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kill Bill: Vol, 1 (2003)</t>
+          <t>Lord of the Rings: The Return of the King, The (2003)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-0.0005175094304871938</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>0.493879</v>
+        <v>-0.17195</v>
       </c>
       <c r="E7" t="n">
-        <v>0.146538</v>
+        <v>0.304292</v>
       </c>
       <c r="F7" t="n">
-        <v>1.327262</v>
+        <v>-0.547663</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.048778</v>
+        <v>-1.16954</v>
       </c>
       <c r="H7" t="n">
-        <v>-0.071466</v>
+        <v>1.095531</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.545494</v>
+        <v>0.26373</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Eternal Sunshine of the Spotless Mind (2004)</t>
+          <t>Monsters, Inc, (2001)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-0.001027513246670205</v>
+        <v>9</v>
       </c>
       <c r="D8" t="n">
-        <v>0.061169</v>
+        <v>-0.143442</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.756446</v>
+        <v>-0.449182</v>
       </c>
       <c r="F8" t="n">
-        <v>1.145716</v>
+        <v>-0.1924</v>
       </c>
       <c r="G8" t="n">
-        <v>0.257291</v>
+        <v>-1.142476</v>
       </c>
       <c r="H8" t="n">
-        <v>0.391489</v>
+        <v>-0.218573</v>
       </c>
       <c r="I8" t="n">
-        <v>0.192423</v>
+        <v>-0.242117</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Twelve Monkeys (a,k,a, 12 Monkeys) (1995)</t>
+          <t>Godfather, The (1972)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.000211202620505321</v>
+        <v>7</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.097064</v>
+        <v>0.586113</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.382386</v>
+        <v>-0.637499</v>
       </c>
       <c r="F9" t="n">
-        <v>0.607228</v>
+        <v>0.92096</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.044485</v>
+        <v>-1.00589</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.229739</v>
+        <v>0.957238</v>
       </c>
       <c r="I9" t="n">
-        <v>0.916936</v>
+        <v>-0.131934</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Memento (2000)</t>
+          <t>Shrek 2 (2004)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0009673798147327878</v>
+        <v>2</v>
       </c>
       <c r="D10" t="n">
-        <v>0.604523</v>
+        <v>0.402436</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.156093</v>
+        <v>-0.444598</v>
       </c>
       <c r="F10" t="n">
-        <v>0.961245</v>
+        <v>-0.602684</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.228593</v>
+        <v>-0.955001</v>
       </c>
       <c r="H10" t="n">
-        <v>0.345702</v>
+        <v>-1.047055</v>
       </c>
       <c r="I10" t="n">
-        <v>0.134959</v>
+        <v>-0.242161</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Raiders of the Lost Ark (Indiana Jones and the Raiders of the Lost Ark) (1981)</t>
+          <t>Finding Nemo (2003)</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.001521532998277525</v>
+        <v>2</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.181312</v>
+        <v>0.288385</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.733017</v>
+        <v>-0.351151</v>
       </c>
       <c r="F11" t="n">
-        <v>0.438087</v>
+        <v>-0.108478</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.49864</v>
+        <v>-0.940476</v>
       </c>
       <c r="H11" t="n">
-        <v>0.979085</v>
+        <v>-0.412718</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.053527</v>
+        <v>-0.808264</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Gladiator (2000)</t>
+          <t>Shawshank Redemption, The (1994)</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-0.04077580432683473</v>
+        <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>0.465508</v>
+        <v>0.596305</v>
       </c>
       <c r="E12" t="n">
-        <v>0.662236</v>
+        <v>0.199528</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.762741</v>
+        <v>0.422264</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.417576</v>
+        <v>-0.897889</v>
       </c>
       <c r="H12" t="n">
-        <v>1.112864</v>
+        <v>1.241398</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.373171</v>
+        <v>0.497348</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Back to the Future (1985)</t>
+          <t>Spider-Man 2 (2004)</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.0002269073633379184</v>
+        <v>1</v>
       </c>
       <c r="D13" t="n">
-        <v>0.257897</v>
+        <v>-0.169168</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.661257</v>
+        <v>-0.275128</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.162848</v>
+        <v>0.193299</v>
       </c>
       <c r="G13" t="n">
-        <v>0.291349</v>
+        <v>-0.838293</v>
       </c>
       <c r="H13" t="n">
-        <v>0.482955</v>
+        <v>-0.905218</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.058067</v>
+        <v>-0.6102610000000001</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Snatch (2000)</t>
+          <t>Shrek (2001)</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.000358303500159235</v>
+        <v>3</v>
       </c>
       <c r="D14" t="n">
-        <v>0.62363</v>
+        <v>0.710371</v>
       </c>
       <c r="E14" t="n">
-        <v>0.194445</v>
+        <v>-0.432438</v>
       </c>
       <c r="F14" t="n">
-        <v>0.449922</v>
+        <v>-0.477484</v>
       </c>
       <c r="G14" t="n">
-        <v>0.439904</v>
+        <v>-0.719125</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.059525</v>
+        <v>-0.276698</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.250803</v>
+        <v>-0.071826</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>99</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Pretty Woman (1990)</t>
+          <t>X2: X-Men United (2003)</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>-3.118480816418847e-05</v>
+        <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>0.035111</v>
+        <v>0.943534</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.047817</v>
+        <v>0.084534</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.462945</v>
+        <v>-0.235003</v>
       </c>
       <c r="G15" t="n">
-        <v>0.09805</v>
+        <v>-0.665734</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.909895</v>
+        <v>-0.94687</v>
       </c>
       <c r="I15" t="n">
-        <v>0.142315</v>
+        <v>-0.378408</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Lord of the Rings: The Fellowship of the Ring, The (2001)</t>
+          <t>Toy Story (1995)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0.005646642482451831</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.225569</v>
+        <v>-0.273328</v>
       </c>
       <c r="E16" t="n">
-        <v>0.240604</v>
+        <v>-0.420326</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.167136</v>
+        <v>-0.480527</v>
       </c>
       <c r="G16" t="n">
-        <v>-1.50213</v>
+        <v>-0.588276</v>
       </c>
       <c r="H16" t="n">
-        <v>1.063062</v>
+        <v>0.365701</v>
       </c>
       <c r="I16" t="n">
-        <v>0.389827</v>
+        <v>-0.467012</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Lord of the Rings: The Two Towers, The (2002)</t>
+          <t>Crouching Tiger, Hidden Dragon (Wo hu cang long) (2000)</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-0.01167958804550444</v>
+        <v>7</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.394141</v>
+        <v>0.395514</v>
       </c>
       <c r="E17" t="n">
-        <v>0.146831</v>
+        <v>-0.371204</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.410531</v>
+        <v>0.728593</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.186645</v>
+        <v>-0.5256459999999999</v>
       </c>
       <c r="H17" t="n">
-        <v>1.096657</v>
+        <v>-0.186908</v>
       </c>
       <c r="I17" t="n">
-        <v>0.377764</v>
+        <v>-0.054575</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Lord of the Rings: The Return of the King, The (2003)</t>
+          <t>V for Vendetta (2006)</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>-0.009682898998743198</v>
+        <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.17195</v>
+        <v>-0.435419</v>
       </c>
       <c r="E18" t="n">
-        <v>0.304292</v>
+        <v>0.382125</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.547663</v>
+        <v>0.308104</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.16954</v>
+        <v>-0.5138239999999999</v>
       </c>
       <c r="H18" t="n">
-        <v>1.095531</v>
+        <v>0.189036</v>
       </c>
       <c r="I18" t="n">
-        <v>0.26373</v>
+        <v>-0.156506</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>O Brother, Where Art Thou? (2000)</t>
+          <t>Chicken Run (2000)</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.02256660625590474</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>1.295014</v>
+        <v>0.089708</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.93472</v>
+        <v>-1.196121</v>
       </c>
       <c r="F19" t="n">
-        <v>0.80421</v>
+        <v>-0.289824</v>
       </c>
       <c r="G19" t="n">
-        <v>0.123279</v>
+        <v>-0.499809</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.549067</v>
+        <v>-0.83693</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.342473</v>
+        <v>-0.420221</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Donnie Darko (2001)</t>
+          <t>Raiders of the Lost Ark (Indiana Jones and the Raiders of the Lost Ark) (1981)</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.006046065780896987</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>0.517054</v>
+        <v>-0.181312</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.171271</v>
+        <v>-0.733017</v>
       </c>
       <c r="F20" t="n">
-        <v>0.892353</v>
+        <v>0.438087</v>
       </c>
       <c r="G20" t="n">
-        <v>0.456009</v>
+        <v>-0.49864</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.563917</v>
+        <v>0.979085</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.297528</v>
+        <v>-0.053527</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Crouching Tiger, Hidden Dragon (Wo hu cang long) (2000)</t>
+          <t>High Fidelity (2000)</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.0005735542488282282</v>
+        <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>0.395514</v>
+        <v>0.359374</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.371204</v>
+        <v>-0.630769</v>
       </c>
       <c r="F21" t="n">
-        <v>0.728593</v>
+        <v>0.623014</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.5256459999999999</v>
+        <v>-0.493241</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.186908</v>
+        <v>-0.689554</v>
       </c>
       <c r="I21" t="n">
-        <v>-0.054575</v>
+        <v>-0.051236</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Lost in Translation (2003)</t>
+          <t>Minority Report (2002)</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>2.76684392343586e-05</v>
+        <v>4</v>
       </c>
       <c r="D22" t="n">
-        <v>0.287842</v>
+        <v>-0.034068</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.207892</v>
+        <v>0.230176</v>
       </c>
       <c r="F22" t="n">
-        <v>1.298714</v>
+        <v>-0.709613</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.002462</v>
+        <v>-0.469021</v>
       </c>
       <c r="H22" t="n">
-        <v>-1.435582</v>
+        <v>0.031316</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.100731</v>
+        <v>0.116521</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Dark Knight, The (2008)</t>
+          <t>Matrix Reloaded, The (2003)</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>-0.01609363165560362</v>
+        <v>1</v>
       </c>
       <c r="D23" t="n">
-        <v>-0.362395</v>
+        <v>-0.108205</v>
       </c>
       <c r="E23" t="n">
-        <v>0.441177</v>
+        <v>0.45824</v>
       </c>
       <c r="F23" t="n">
-        <v>0.460574</v>
+        <v>-1.22588</v>
       </c>
       <c r="G23" t="n">
-        <v>0.296781</v>
+        <v>-0.468387</v>
       </c>
       <c r="H23" t="n">
-        <v>0.745397</v>
+        <v>-0.97848</v>
       </c>
       <c r="I23" t="n">
-        <v>0.9879520000000001</v>
+        <v>0.040841</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Ocean's Eleven (2001)</t>
+          <t>Cast Away (2000)</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.000526595803532445</v>
+        <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>0.551612</v>
+        <v>1.014575</v>
       </c>
       <c r="E24" t="n">
-        <v>0.185851</v>
+        <v>0.403793</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.3449</v>
+        <v>-0.477961</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.21897</v>
+        <v>-0.450861</v>
       </c>
       <c r="H24" t="n">
-        <v>0.128355</v>
+        <v>0.355866</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.5298929999999999</v>
+        <v>-1.331613</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Minority Report (2002)</t>
+          <t>Sixth Sense, The (1999)</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>-9.523377858349936e-06</v>
+        <v>9</v>
       </c>
       <c r="D25" t="n">
-        <v>-0.034068</v>
+        <v>0.546339</v>
       </c>
       <c r="E25" t="n">
-        <v>0.230176</v>
+        <v>0.06449199999999999</v>
       </c>
       <c r="F25" t="n">
-        <v>-0.709613</v>
+        <v>0.045092</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.469021</v>
+        <v>-0.448679</v>
       </c>
       <c r="H25" t="n">
-        <v>0.031316</v>
+        <v>0.340016</v>
       </c>
       <c r="I25" t="n">
-        <v>0.116521</v>
+        <v>0.060574</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sin City (2005)</t>
+          <t>Gladiator (2000)</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>-0.1073574500772207</v>
+        <v>7</v>
       </c>
       <c r="D26" t="n">
-        <v>-1.174844</v>
+        <v>0.465508</v>
       </c>
       <c r="E26" t="n">
-        <v>1.34822</v>
+        <v>0.662236</v>
       </c>
       <c r="F26" t="n">
-        <v>0.570489</v>
+        <v>-0.762741</v>
       </c>
       <c r="G26" t="n">
-        <v>0.283971</v>
+        <v>-0.417576</v>
       </c>
       <c r="H26" t="n">
-        <v>-0.42946</v>
+        <v>1.112864</v>
       </c>
       <c r="I26" t="n">
-        <v>-0.974198</v>
+        <v>-0.373171</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Amelie (2001)</t>
+          <t>Fargo (1996)</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.0008075564936502852</v>
+        <v>2</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.350705</v>
+        <v>0.136574</v>
       </c>
       <c r="E27" t="n">
-        <v>0.13062</v>
+        <v>-0.091109</v>
       </c>
       <c r="F27" t="n">
-        <v>1.027575</v>
+        <v>0.5009479999999999</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.07173400000000001</v>
+        <v>-0.407633</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.430135</v>
+        <v>0.088792</v>
       </c>
       <c r="I27" t="n">
-        <v>-0.5560040000000001</v>
+        <v>0.326508</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Braveheart (1995)</t>
+          <t>Silence of the Lambs, The (1991)</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.002707486004041554</v>
+        <v>1</v>
       </c>
       <c r="D28" t="n">
-        <v>1.003499</v>
+        <v>0.249822</v>
       </c>
       <c r="E28" t="n">
-        <v>0.259038</v>
+        <v>-0.202331</v>
       </c>
       <c r="F28" t="n">
-        <v>-0.173291</v>
+        <v>0.443764</v>
       </c>
       <c r="G28" t="n">
-        <v>-0.266258</v>
+        <v>-0.382624</v>
       </c>
       <c r="H28" t="n">
-        <v>0.785951</v>
+        <v>0.300838</v>
       </c>
       <c r="I28" t="n">
-        <v>0.287218</v>
+        <v>0.446762</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Godfather, The (1972)</t>
+          <t>Spider-Man (2002)</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-0.04371482870438264</v>
+        <v>5</v>
       </c>
       <c r="D29" t="n">
-        <v>0.586113</v>
+        <v>0.145272</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.637499</v>
+        <v>0.175034</v>
       </c>
       <c r="F29" t="n">
-        <v>0.92096</v>
+        <v>-0.133207</v>
       </c>
       <c r="G29" t="n">
-        <v>-1.00589</v>
+        <v>-0.380053</v>
       </c>
       <c r="H29" t="n">
-        <v>0.957238</v>
+        <v>-0.695503</v>
       </c>
       <c r="I29" t="n">
-        <v>-0.131934</v>
+        <v>-0.728745</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>84</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>High Fidelity (2000)</t>
+          <t>Bourne Identity, The (2002)</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.002461033182303874</v>
+        <v>3</v>
       </c>
       <c r="D30" t="n">
-        <v>0.359374</v>
+        <v>0.266225</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.630769</v>
+        <v>0.500795</v>
       </c>
       <c r="F30" t="n">
-        <v>0.623014</v>
+        <v>-0.162073</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.493241</v>
+        <v>-0.345967</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.689554</v>
+        <v>0.059598</v>
       </c>
       <c r="I30" t="n">
-        <v>-0.051236</v>
+        <v>-0.095469</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Batman (1989)</t>
+          <t>Rock, The (1996)</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>-0.0001566305655461317</v>
+        <v>7</v>
       </c>
       <c r="D31" t="n">
-        <v>0.524029</v>
+        <v>0.139304</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.148073</v>
+        <v>-0.48713</v>
       </c>
       <c r="F31" t="n">
-        <v>0.013642</v>
+        <v>-0.7407049999999999</v>
       </c>
       <c r="G31" t="n">
-        <v>0.54508</v>
+        <v>-0.303868</v>
       </c>
       <c r="H31" t="n">
-        <v>-0.6282489999999999</v>
+        <v>-0.449029</v>
       </c>
       <c r="I31" t="n">
-        <v>-0.432091</v>
+        <v>-0.103806</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Batman Begins (2005)</t>
+          <t>Matrix, The (1999)</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-7.533162075366106e-06</v>
+        <v>7</v>
       </c>
       <c r="D32" t="n">
-        <v>-0.311075</v>
+        <v>-0.971155</v>
       </c>
       <c r="E32" t="n">
-        <v>0.161113</v>
+        <v>0.032008</v>
       </c>
       <c r="F32" t="n">
-        <v>0.199317</v>
+        <v>0.113094</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.285839</v>
+        <v>-0.288342</v>
       </c>
       <c r="H32" t="n">
-        <v>0.597024</v>
+        <v>1.009168</v>
       </c>
       <c r="I32" t="n">
-        <v>-0.004419</v>
+        <v>1.258047</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Silence of the Lambs, The (1991)</t>
+          <t>Batman Begins (2005)</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.001153523119226829</v>
+        <v>7</v>
       </c>
       <c r="D33" t="n">
-        <v>0.249822</v>
+        <v>-0.311075</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.202331</v>
+        <v>0.161113</v>
       </c>
       <c r="F33" t="n">
-        <v>0.443764</v>
+        <v>0.199317</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.382624</v>
+        <v>-0.285839</v>
       </c>
       <c r="H33" t="n">
-        <v>0.300838</v>
+        <v>0.597024</v>
       </c>
       <c r="I33" t="n">
-        <v>0.446762</v>
+        <v>-0.004419</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Fargo (1996)</t>
+          <t>Patriot, The (2000)</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>7.366462060775738e-05</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>0.136574</v>
+        <v>0.804366</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.091109</v>
+        <v>-0.246102</v>
       </c>
       <c r="F34" t="n">
-        <v>0.5009479999999999</v>
+        <v>-1.203248</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.407633</v>
+        <v>-0.282312</v>
       </c>
       <c r="H34" t="n">
-        <v>0.088792</v>
+        <v>-0.291594</v>
       </c>
       <c r="I34" t="n">
-        <v>0.326508</v>
+        <v>-0.234564</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Shawshank Redemption, The (1994)</t>
+          <t>Catch Me If You Can (2002)</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.02785161773866425</v>
+        <v>7</v>
       </c>
       <c r="D35" t="n">
-        <v>0.596305</v>
+        <v>1.205988</v>
       </c>
       <c r="E35" t="n">
-        <v>0.199528</v>
+        <v>0.509645</v>
       </c>
       <c r="F35" t="n">
-        <v>0.422264</v>
+        <v>-0.262317</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.897889</v>
+        <v>-0.274633</v>
       </c>
       <c r="H35" t="n">
-        <v>1.241398</v>
+        <v>0.242309</v>
       </c>
       <c r="I35" t="n">
-        <v>0.497348</v>
+        <v>0.819855</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Terminator 2: Judgment Day (1991)</t>
+          <t>Requiem for a Dream (2000)</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3.186882519605924e-05</v>
+        <v>8</v>
       </c>
       <c r="D36" t="n">
-        <v>0.027123</v>
+        <v>-0.139526</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.178035</v>
+        <v>0.620814</v>
       </c>
       <c r="F36" t="n">
-        <v>-0.365473</v>
+        <v>1.210166</v>
       </c>
       <c r="G36" t="n">
-        <v>0.552849</v>
+        <v>-0.269602</v>
       </c>
       <c r="H36" t="n">
-        <v>0.199415</v>
+        <v>-0.179697</v>
       </c>
       <c r="I36" t="n">
-        <v>0.163796</v>
+        <v>0.392308</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Jurassic Park (1993)</t>
+          <t>Braveheart (1995)</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-6.47918598268611e-07</v>
+        <v>9</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.005639</v>
+        <v>1.003499</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.297029</v>
+        <v>0.259038</v>
       </c>
       <c r="F37" t="n">
-        <v>-0.780308</v>
+        <v>-0.173291</v>
       </c>
       <c r="G37" t="n">
-        <v>0.098915</v>
+        <v>-0.266258</v>
       </c>
       <c r="H37" t="n">
-        <v>-0.015127</v>
+        <v>0.785951</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.331313</v>
+        <v>0.287218</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Kill Bill: Vol, 2 (2004)</t>
+          <t>Memento (2000)</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.0122956430641111</v>
+        <v>8</v>
       </c>
       <c r="D38" t="n">
-        <v>0.68703</v>
+        <v>0.604523</v>
       </c>
       <c r="E38" t="n">
-        <v>0.073925</v>
+        <v>-0.156093</v>
       </c>
       <c r="F38" t="n">
-        <v>1.732061</v>
+        <v>0.961245</v>
       </c>
       <c r="G38" t="n">
-        <v>0.449929</v>
+        <v>-0.228593</v>
       </c>
       <c r="H38" t="n">
-        <v>-0.18962</v>
+        <v>0.345702</v>
       </c>
       <c r="I38" t="n">
-        <v>-1.638298</v>
+        <v>0.134959</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Batman Forever (1995)</t>
+          <t>Saving Private Ryan (1998)</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>-9.688510852033622e-05</v>
+        <v>4</v>
       </c>
       <c r="D39" t="n">
-        <v>0.087715</v>
+        <v>0.234844</v>
       </c>
       <c r="E39" t="n">
-        <v>0.004544</v>
+        <v>1.100681</v>
       </c>
       <c r="F39" t="n">
-        <v>-1.690647</v>
+        <v>-0.106135</v>
       </c>
       <c r="G39" t="n">
-        <v>0.301528</v>
+        <v>-0.221473</v>
       </c>
       <c r="H39" t="n">
-        <v>-1.182924</v>
+        <v>0.698416</v>
       </c>
       <c r="I39" t="n">
-        <v>-0.403095</v>
+        <v>-0.158787</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Schindler's List (1993)</t>
+          <t>Ocean's Eleven (2001)</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>-3.049962597159831e-05</v>
+        <v>6</v>
       </c>
       <c r="D40" t="n">
-        <v>0.469902</v>
+        <v>0.551612</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.059721</v>
+        <v>0.185851</v>
       </c>
       <c r="F40" t="n">
-        <v>0.172039</v>
+        <v>-0.3449</v>
       </c>
       <c r="G40" t="n">
-        <v>-1.389097</v>
+        <v>-0.21897</v>
       </c>
       <c r="H40" t="n">
-        <v>0.56819</v>
+        <v>0.128355</v>
       </c>
       <c r="I40" t="n">
-        <v>-0.008004000000000001</v>
+        <v>-0.5298929999999999</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Beautiful Mind, A (2001)</t>
+          <t>Seven (a,k,a, Se7en) (1995)</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>9.726135381498439e-05</v>
+        <v>2</v>
       </c>
       <c r="D41" t="n">
-        <v>0.728008</v>
+        <v>0.095857</v>
       </c>
       <c r="E41" t="n">
-        <v>0.448111</v>
+        <v>0.117969</v>
       </c>
       <c r="F41" t="n">
-        <v>0.155385</v>
+        <v>0.435691</v>
       </c>
       <c r="G41" t="n">
-        <v>0.026203</v>
+        <v>-0.153376</v>
       </c>
       <c r="H41" t="n">
-        <v>0.427099</v>
+        <v>0.262826</v>
       </c>
       <c r="I41" t="n">
-        <v>0.171447</v>
+        <v>0.732908</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Erin Brockovich (2000)</t>
+          <t>E,T, the Extra-Terrestrial (1982)</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.006205360261983062</v>
+        <v>8</v>
       </c>
       <c r="D42" t="n">
-        <v>1.581845</v>
+        <v>0.697551</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.62645</v>
+        <v>-0.648977</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.213707</v>
+        <v>-0.558817</v>
       </c>
       <c r="G42" t="n">
-        <v>0.343191</v>
+        <v>-0.138365</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.639564</v>
+        <v>0.499346</v>
       </c>
       <c r="I42" t="n">
-        <v>-0.133499</v>
+        <v>-0.131174</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Fight Club (1999)</t>
+          <t>Pulp Fiction (1994)</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>-0.0407523517290936</v>
+        <v>4</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.289515</v>
+        <v>0.059799</v>
       </c>
       <c r="E43" t="n">
-        <v>0.565428</v>
+        <v>-0.079411</v>
       </c>
       <c r="F43" t="n">
-        <v>1.511413</v>
+        <v>1.442504</v>
       </c>
       <c r="G43" t="n">
-        <v>0.8930399999999999</v>
+        <v>-0.138159</v>
       </c>
       <c r="H43" t="n">
-        <v>0.252663</v>
+        <v>0.050682</v>
       </c>
       <c r="I43" t="n">
-        <v>0.729976</v>
+        <v>0.401355</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Spider-Man (2002)</t>
+          <t>Mrs, Doubtfire (1993)</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.0006524543658968464</v>
+        <v>7</v>
       </c>
       <c r="D44" t="n">
-        <v>0.145272</v>
+        <v>0.561999</v>
       </c>
       <c r="E44" t="n">
-        <v>0.175034</v>
+        <v>-0.107344</v>
       </c>
       <c r="F44" t="n">
-        <v>-0.133207</v>
+        <v>-1.654256</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.380053</v>
+        <v>-0.112372</v>
       </c>
       <c r="H44" t="n">
-        <v>-0.695503</v>
+        <v>-0.64331</v>
       </c>
       <c r="I44" t="n">
-        <v>-0.728745</v>
+        <v>-0.106764</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Spider-Man 2 (2004)</t>
+          <t>American Beauty (1999)</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>-0.004166268455748494</v>
+        <v>8</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.169168</v>
+        <v>-0.04848</v>
       </c>
       <c r="E45" t="n">
-        <v>-0.275128</v>
+        <v>0.126738</v>
       </c>
       <c r="F45" t="n">
-        <v>0.193299</v>
+        <v>0.46106</v>
       </c>
       <c r="G45" t="n">
-        <v>-0.838293</v>
+        <v>-0.10675</v>
       </c>
       <c r="H45" t="n">
-        <v>-0.905218</v>
+        <v>0.39937</v>
       </c>
       <c r="I45" t="n">
-        <v>-0.6102610000000001</v>
+        <v>0.399536</v>
       </c>
     </row>
     <row r="46">
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>-0.0002509797605762717</v>
+        <v>6</v>
       </c>
       <c r="D46" t="n">
         <v>0.545602</v>
@@ -1877,1707 +1877,1707 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Dances with Wolves (1990)</t>
+          <t>Departed, The (2006)</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.202839721696942e-05</v>
+        <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.42137</v>
+        <v>0.875568</v>
       </c>
       <c r="E47" t="n">
-        <v>0.034947</v>
+        <v>-0.319582</v>
       </c>
       <c r="F47" t="n">
-        <v>-0.676508</v>
+        <v>0.462147</v>
       </c>
       <c r="G47" t="n">
-        <v>0.09578399999999999</v>
+        <v>-0.07702199999999999</v>
       </c>
       <c r="H47" t="n">
-        <v>0.055122</v>
+        <v>0.89249</v>
       </c>
       <c r="I47" t="n">
-        <v>-0.228688</v>
+        <v>0.245303</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Monsters, Inc, (2001)</t>
+          <t>Amelie (2001)</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.0007495017082049324</v>
+        <v>7</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.143442</v>
+        <v>-0.350705</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.449182</v>
+        <v>0.13062</v>
       </c>
       <c r="F48" t="n">
-        <v>-0.1924</v>
+        <v>1.027575</v>
       </c>
       <c r="G48" t="n">
-        <v>-1.142476</v>
+        <v>-0.07173400000000001</v>
       </c>
       <c r="H48" t="n">
-        <v>-0.218573</v>
+        <v>-0.430135</v>
       </c>
       <c r="I48" t="n">
-        <v>-0.242117</v>
+        <v>-0.5560040000000001</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Titanic (1997)</t>
+          <t>Meet the Parents (2000)</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>-7.13409225881008e-05</v>
+        <v>6</v>
       </c>
       <c r="D49" t="n">
-        <v>0.682626</v>
+        <v>0.234633</v>
       </c>
       <c r="E49" t="n">
-        <v>0.344819</v>
+        <v>-0.364501</v>
       </c>
       <c r="F49" t="n">
-        <v>-1.513952</v>
+        <v>-0.705371</v>
       </c>
       <c r="G49" t="n">
-        <v>0.082233</v>
+        <v>-0.069191</v>
       </c>
       <c r="H49" t="n">
-        <v>-0.280083</v>
+        <v>-0.561307</v>
       </c>
       <c r="I49" t="n">
-        <v>-0.008692</v>
+        <v>-0.221236</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>E,T, the Extra-Terrestrial (1982)</t>
+          <t>Kill Bill: Vol, 1 (2003)</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.002292717075288345</v>
+        <v>2</v>
       </c>
       <c r="D50" t="n">
-        <v>0.697551</v>
+        <v>0.493879</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.648977</v>
+        <v>0.146538</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.558817</v>
+        <v>1.327262</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.138365</v>
+        <v>-0.048778</v>
       </c>
       <c r="H50" t="n">
-        <v>0.499346</v>
+        <v>-0.071466</v>
       </c>
       <c r="I50" t="n">
-        <v>-0.131174</v>
+        <v>-1.545494</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Independence Day (a,k,a, ID4) (1996)</t>
+          <t>Twelve Monkeys (a,k,a, 12 Monkeys) (1995)</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.07259577658048338</v>
+        <v>5</v>
       </c>
       <c r="D51" t="n">
-        <v>0.385232</v>
+        <v>-0.097064</v>
       </c>
       <c r="E51" t="n">
-        <v>-0.440648</v>
+        <v>-0.382386</v>
       </c>
       <c r="F51" t="n">
-        <v>-1.013302</v>
+        <v>0.607228</v>
       </c>
       <c r="G51" t="n">
-        <v>0.733044</v>
+        <v>-0.044485</v>
       </c>
       <c r="H51" t="n">
-        <v>-0.587827</v>
+        <v>-0.229739</v>
       </c>
       <c r="I51" t="n">
-        <v>-0.979442</v>
+        <v>0.916936</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>51</v>
+        <v>72</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Matrix, The (1999)</t>
+          <t>Mission: Impossible (1996)</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.001286929918575478</v>
+        <v>2</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.971155</v>
+        <v>-0.065584</v>
       </c>
       <c r="E52" t="n">
-        <v>0.032008</v>
+        <v>-0.760031</v>
       </c>
       <c r="F52" t="n">
-        <v>0.113094</v>
+        <v>-0.962643</v>
       </c>
       <c r="G52" t="n">
-        <v>-0.288342</v>
+        <v>-0.033056</v>
       </c>
       <c r="H52" t="n">
-        <v>1.009168</v>
+        <v>-0.657868</v>
       </c>
       <c r="I52" t="n">
-        <v>1.258047</v>
+        <v>0.151277</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Matrix Reloaded, The (2003)</t>
+          <t>Forrest Gump (1994)</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.001137735838800648</v>
+        <v>9</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.108205</v>
+        <v>0.901322</v>
       </c>
       <c r="E53" t="n">
-        <v>0.45824</v>
+        <v>0.865292</v>
       </c>
       <c r="F53" t="n">
-        <v>-1.22588</v>
+        <v>-0.037117</v>
       </c>
       <c r="G53" t="n">
-        <v>-0.468387</v>
+        <v>-0.026354</v>
       </c>
       <c r="H53" t="n">
-        <v>-0.97848</v>
+        <v>0.988768</v>
       </c>
       <c r="I53" t="n">
-        <v>0.040841</v>
+        <v>-0.024578</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Men in Black (a,k,a, MIB) (1997)</t>
+          <t>Twister (1996)</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0.002866224555402718</v>
+        <v>5</v>
       </c>
       <c r="D54" t="n">
-        <v>0.282286</v>
+        <v>0.422157</v>
       </c>
       <c r="E54" t="n">
-        <v>-0.583039</v>
+        <v>-0.553928</v>
       </c>
       <c r="F54" t="n">
-        <v>-0.5789029999999999</v>
+        <v>-1.847263</v>
       </c>
       <c r="G54" t="n">
-        <v>0.268523</v>
+        <v>-0.025584</v>
       </c>
       <c r="H54" t="n">
-        <v>-0.585829</v>
+        <v>-1.160915</v>
       </c>
       <c r="I54" t="n">
-        <v>-0.191234</v>
+        <v>0.042537</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Usual Suspects, The (1995)</t>
+          <t>X-Men (2000)</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5.749141069120103e-05</v>
+        <v>6</v>
       </c>
       <c r="D55" t="n">
-        <v>0.70496</v>
+        <v>0.471031</v>
       </c>
       <c r="E55" t="n">
-        <v>-0.058955</v>
+        <v>-0.20257</v>
       </c>
       <c r="F55" t="n">
-        <v>1.01613</v>
+        <v>-0.10811</v>
       </c>
       <c r="G55" t="n">
-        <v>-0.004273</v>
+        <v>-0.02124</v>
       </c>
       <c r="H55" t="n">
-        <v>0.33338</v>
+        <v>-0.8985</v>
       </c>
       <c r="I55" t="n">
-        <v>0.955644</v>
+        <v>-0.42079</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Catch Me If You Can (2002)</t>
+          <t>Usual Suspects, The (1995)</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.008796228591580475</v>
+        <v>3</v>
       </c>
       <c r="D56" t="n">
-        <v>1.205988</v>
+        <v>0.70496</v>
       </c>
       <c r="E56" t="n">
-        <v>0.509645</v>
+        <v>-0.058955</v>
       </c>
       <c r="F56" t="n">
-        <v>-0.262317</v>
+        <v>1.01613</v>
       </c>
       <c r="G56" t="n">
-        <v>-0.274633</v>
+        <v>-0.004273</v>
       </c>
       <c r="H56" t="n">
-        <v>0.242309</v>
+        <v>0.33338</v>
       </c>
       <c r="I56" t="n">
-        <v>0.819855</v>
+        <v>0.955644</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Requiem for a Dream (2000)</t>
+          <t>Lost in Translation (2003)</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>-0.001992290636683343</v>
+        <v>4</v>
       </c>
       <c r="D57" t="n">
-        <v>-0.139526</v>
+        <v>0.287842</v>
       </c>
       <c r="E57" t="n">
-        <v>0.620814</v>
+        <v>-0.207892</v>
       </c>
       <c r="F57" t="n">
-        <v>1.210166</v>
+        <v>1.298714</v>
       </c>
       <c r="G57" t="n">
-        <v>-0.269602</v>
+        <v>-0.002462</v>
       </c>
       <c r="H57" t="n">
-        <v>-0.179697</v>
+        <v>-1.435582</v>
       </c>
       <c r="I57" t="n">
-        <v>0.392308</v>
+        <v>-0.100731</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Twister (1996)</t>
+          <t>Beautiful Mind, A (2001)</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.0005457475205121235</v>
+        <v>3</v>
       </c>
       <c r="D58" t="n">
-        <v>0.422157</v>
+        <v>0.728008</v>
       </c>
       <c r="E58" t="n">
-        <v>-0.553928</v>
+        <v>0.448111</v>
       </c>
       <c r="F58" t="n">
-        <v>-1.847263</v>
+        <v>0.155385</v>
       </c>
       <c r="G58" t="n">
-        <v>-0.025584</v>
+        <v>0.026203</v>
       </c>
       <c r="H58" t="n">
-        <v>-1.160915</v>
+        <v>0.427099</v>
       </c>
       <c r="I58" t="n">
-        <v>0.042537</v>
+        <v>0.171447</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Harry Potter and the Sorcerer's Stone (a,k,a, Harry Potter and the Philosopher's Stone) (2001)</t>
+          <t>Fugitive, The (1993)</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>-0.003186048881480703</v>
+        <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>1.359601</v>
+        <v>0.399062</v>
       </c>
       <c r="E59" t="n">
-        <v>0.07443900000000001</v>
+        <v>-0.6332140000000001</v>
       </c>
       <c r="F59" t="n">
-        <v>-0.668836</v>
+        <v>-0.5366030000000001</v>
       </c>
       <c r="G59" t="n">
-        <v>0.532676</v>
+        <v>0.065729</v>
       </c>
       <c r="H59" t="n">
-        <v>-0.447798</v>
+        <v>0.158757</v>
       </c>
       <c r="I59" t="n">
-        <v>-0.197322</v>
+        <v>0.542654</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Harry Potter and the Chamber of Secrets (2002)</t>
+          <t>Titanic (1997)</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>-0.01584880284494024</v>
+        <v>9</v>
       </c>
       <c r="D60" t="n">
-        <v>1.426698</v>
+        <v>0.682626</v>
       </c>
       <c r="E60" t="n">
-        <v>-0.729712</v>
+        <v>0.344819</v>
       </c>
       <c r="F60" t="n">
-        <v>-0.290322</v>
+        <v>-1.513952</v>
       </c>
       <c r="G60" t="n">
-        <v>0.197229</v>
+        <v>0.082233</v>
       </c>
       <c r="H60" t="n">
-        <v>-0.392079</v>
+        <v>-0.280083</v>
       </c>
       <c r="I60" t="n">
-        <v>0.678092</v>
+        <v>-0.008692</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Pulp Fiction (1994)</t>
+          <t>Star Wars: Episode V - The Empire Strikes Back (1980)</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1.925099654138624e-05</v>
+        <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>0.059799</v>
+        <v>-0.647379</v>
       </c>
       <c r="E61" t="n">
-        <v>-0.079411</v>
+        <v>-0.566604</v>
       </c>
       <c r="F61" t="n">
-        <v>1.442504</v>
+        <v>0.349584</v>
       </c>
       <c r="G61" t="n">
-        <v>-0.138159</v>
+        <v>0.082728</v>
       </c>
       <c r="H61" t="n">
-        <v>0.050682</v>
+        <v>1.256632</v>
       </c>
       <c r="I61" t="n">
-        <v>0.401355</v>
+        <v>-0.747074</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Sixth Sense, The (1999)</t>
+          <t>Speed (1994)</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>-1.468212433230657e-05</v>
+        <v>2</v>
       </c>
       <c r="D62" t="n">
-        <v>0.546339</v>
+        <v>0.135632</v>
       </c>
       <c r="E62" t="n">
-        <v>0.06449199999999999</v>
+        <v>-0.647521</v>
       </c>
       <c r="F62" t="n">
-        <v>0.045092</v>
+        <v>-1.55715</v>
       </c>
       <c r="G62" t="n">
-        <v>-0.448679</v>
+        <v>0.094816</v>
       </c>
       <c r="H62" t="n">
-        <v>0.340016</v>
+        <v>-0.480833</v>
       </c>
       <c r="I62" t="n">
-        <v>0.060574</v>
+        <v>0.658863</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>V for Vendetta (2006)</t>
+          <t>Dances with Wolves (1990)</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>-0.0007792917184337799</v>
+        <v>2</v>
       </c>
       <c r="D63" t="n">
-        <v>-0.435419</v>
+        <v>0.42137</v>
       </c>
       <c r="E63" t="n">
-        <v>0.382125</v>
+        <v>0.034947</v>
       </c>
       <c r="F63" t="n">
-        <v>0.308104</v>
+        <v>-0.676508</v>
       </c>
       <c r="G63" t="n">
-        <v>-0.5138239999999999</v>
+        <v>0.09578399999999999</v>
       </c>
       <c r="H63" t="n">
-        <v>0.189036</v>
+        <v>0.055122</v>
       </c>
       <c r="I63" t="n">
-        <v>-0.156506</v>
+        <v>-0.228688</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Almost Famous (2000)</t>
+          <t>Pretty Woman (1990)</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>-8.896784488522345e-05</v>
+        <v>9</v>
       </c>
       <c r="D64" t="n">
-        <v>0.618167</v>
+        <v>0.035111</v>
       </c>
       <c r="E64" t="n">
-        <v>0.041198</v>
+        <v>-0.047817</v>
       </c>
       <c r="F64" t="n">
-        <v>-0.129813</v>
+        <v>-1.462945</v>
       </c>
       <c r="G64" t="n">
-        <v>0.388409</v>
+        <v>0.09805</v>
       </c>
       <c r="H64" t="n">
-        <v>0.182649</v>
+        <v>-0.909895</v>
       </c>
       <c r="I64" t="n">
-        <v>0.379338</v>
+        <v>0.142315</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Mrs, Doubtfire (1993)</t>
+          <t>Jurassic Park (1993)</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>-0.000770227969743642</v>
+        <v>2</v>
       </c>
       <c r="D65" t="n">
-        <v>0.561999</v>
+        <v>-0.005639</v>
       </c>
       <c r="E65" t="n">
-        <v>-0.107344</v>
+        <v>-0.297029</v>
       </c>
       <c r="F65" t="n">
-        <v>-1.654256</v>
+        <v>-0.780308</v>
       </c>
       <c r="G65" t="n">
-        <v>-0.112372</v>
+        <v>0.098915</v>
       </c>
       <c r="H65" t="n">
-        <v>-0.64331</v>
+        <v>-0.015127</v>
       </c>
       <c r="I65" t="n">
-        <v>-0.106764</v>
+        <v>-0.331313</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Seven (a,k,a, Se7en) (1995)</t>
+          <t>Star Wars: Episode II - Attack of the Clones (2002)</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>-0.0001455611623259159</v>
+        <v>3</v>
       </c>
       <c r="D66" t="n">
-        <v>0.095857</v>
+        <v>1.052404</v>
       </c>
       <c r="E66" t="n">
-        <v>0.117969</v>
+        <v>0.753224</v>
       </c>
       <c r="F66" t="n">
-        <v>0.435691</v>
+        <v>-1.531839</v>
       </c>
       <c r="G66" t="n">
-        <v>-0.153376</v>
+        <v>0.09943</v>
       </c>
       <c r="H66" t="n">
-        <v>0.262826</v>
+        <v>-0.746401</v>
       </c>
       <c r="I66" t="n">
-        <v>0.732908</v>
+        <v>-0.7899</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Shrek (2001)</t>
+          <t>O Brother, Where Art Thou? (2000)</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>-0.002096331621409923</v>
+        <v>1</v>
       </c>
       <c r="D67" t="n">
-        <v>0.710371</v>
+        <v>1.295014</v>
       </c>
       <c r="E67" t="n">
-        <v>-0.432438</v>
+        <v>-0.93472</v>
       </c>
       <c r="F67" t="n">
-        <v>-0.477484</v>
+        <v>0.80421</v>
       </c>
       <c r="G67" t="n">
-        <v>-0.719125</v>
+        <v>0.123279</v>
       </c>
       <c r="H67" t="n">
-        <v>-0.276698</v>
+        <v>-0.549067</v>
       </c>
       <c r="I67" t="n">
-        <v>-0.071826</v>
+        <v>-0.342473</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Shrek 2 (2004)</t>
+          <t>Clear and Present Danger (1994)</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>-0.02611148149074605</v>
+        <v>2</v>
       </c>
       <c r="D68" t="n">
-        <v>0.402436</v>
+        <v>0.521285</v>
       </c>
       <c r="E68" t="n">
-        <v>-0.444598</v>
+        <v>-0.234548</v>
       </c>
       <c r="F68" t="n">
-        <v>-0.602684</v>
+        <v>-0.772875</v>
       </c>
       <c r="G68" t="n">
-        <v>-0.955001</v>
+        <v>0.154113</v>
       </c>
       <c r="H68" t="n">
-        <v>-1.047055</v>
+        <v>-0.073448</v>
       </c>
       <c r="I68" t="n">
-        <v>-0.242161</v>
+        <v>-0.068948</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Aladdin (1992)</t>
+          <t>Charlie's Angels (2000)</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>-0.001589801769783398</v>
+        <v>1</v>
       </c>
       <c r="D69" t="n">
-        <v>0.748726</v>
+        <v>0.665559</v>
       </c>
       <c r="E69" t="n">
-        <v>-0.85102</v>
+        <v>-0.472255</v>
       </c>
       <c r="F69" t="n">
-        <v>-0.638213</v>
+        <v>-1.249498</v>
       </c>
       <c r="G69" t="n">
-        <v>0.26644</v>
+        <v>0.18608</v>
       </c>
       <c r="H69" t="n">
-        <v>0.051811</v>
+        <v>-1.503001</v>
       </c>
       <c r="I69" t="n">
-        <v>-0.2832</v>
+        <v>-0.950063</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Mask, The (1994)</t>
+          <t>Harry Potter and the Chamber of Secrets (2002)</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.01314007904167741</v>
+        <v>3</v>
       </c>
       <c r="D70" t="n">
-        <v>0.43985</v>
+        <v>1.426698</v>
       </c>
       <c r="E70" t="n">
-        <v>-0.116494</v>
+        <v>-0.729712</v>
       </c>
       <c r="F70" t="n">
-        <v>-1.091039</v>
+        <v>-0.290322</v>
       </c>
       <c r="G70" t="n">
-        <v>0.636489</v>
+        <v>0.197229</v>
       </c>
       <c r="H70" t="n">
-        <v>-0.856053</v>
+        <v>-0.392079</v>
       </c>
       <c r="I70" t="n">
-        <v>-0.431378</v>
+        <v>0.678092</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Saving Private Ryan (1998)</t>
+          <t>Star Wars: Episode IV - A New Hope (1977)</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>-0.0006738286539562055</v>
+        <v>9</v>
       </c>
       <c r="D71" t="n">
-        <v>0.234844</v>
+        <v>-0.439267</v>
       </c>
       <c r="E71" t="n">
-        <v>1.100681</v>
+        <v>-1.200818</v>
       </c>
       <c r="F71" t="n">
-        <v>-0.106135</v>
+        <v>0.382361</v>
       </c>
       <c r="G71" t="n">
-        <v>-0.221473</v>
+        <v>0.199633</v>
       </c>
       <c r="H71" t="n">
-        <v>0.698416</v>
+        <v>1.058424</v>
       </c>
       <c r="I71" t="n">
-        <v>-0.158787</v>
+        <v>-0.422181</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Toy Story (1995)</t>
+          <t>Star Wars: Episode VI - Return of the Jedi (1983)</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>-0.005546557148653283</v>
+        <v>6</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.273328</v>
+        <v>-0.612156</v>
       </c>
       <c r="E72" t="n">
-        <v>-0.420326</v>
+        <v>-0.8104170000000001</v>
       </c>
       <c r="F72" t="n">
-        <v>-0.480527</v>
+        <v>-0.067179</v>
       </c>
       <c r="G72" t="n">
-        <v>-0.588276</v>
+        <v>0.222448</v>
       </c>
       <c r="H72" t="n">
-        <v>0.365701</v>
+        <v>1.080815</v>
       </c>
       <c r="I72" t="n">
-        <v>-0.467012</v>
+        <v>-0.738045</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Mission: Impossible (1996)</t>
+          <t>Eternal Sunshine of the Spotless Mind (2004)</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>-0.0001578543047731116</v>
+        <v>5</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.065584</v>
+        <v>0.061169</v>
       </c>
       <c r="E73" t="n">
-        <v>-0.760031</v>
+        <v>-0.756446</v>
       </c>
       <c r="F73" t="n">
-        <v>-0.962643</v>
+        <v>1.145716</v>
       </c>
       <c r="G73" t="n">
-        <v>-0.033056</v>
+        <v>0.257291</v>
       </c>
       <c r="H73" t="n">
-        <v>-0.657868</v>
+        <v>0.391489</v>
       </c>
       <c r="I73" t="n">
-        <v>0.151277</v>
+        <v>0.192423</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Mission: Impossible II (2000)</t>
+          <t>Aladdin (1992)</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.04873050157311503</v>
+        <v>2</v>
       </c>
       <c r="D74" t="n">
-        <v>0.538805</v>
+        <v>0.748726</v>
       </c>
       <c r="E74" t="n">
-        <v>-0.211818</v>
+        <v>-0.85102</v>
       </c>
       <c r="F74" t="n">
-        <v>-1.755887</v>
+        <v>-0.638213</v>
       </c>
       <c r="G74" t="n">
-        <v>0.310784</v>
+        <v>0.26644</v>
       </c>
       <c r="H74" t="n">
-        <v>-1.39709</v>
+        <v>0.051811</v>
       </c>
       <c r="I74" t="n">
-        <v>-0.56005</v>
+        <v>-0.2832</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Departed, The (2006)</t>
+          <t>Men in Black (a,k,a, MIB) (1997)</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.002180586600604161</v>
+        <v>2</v>
       </c>
       <c r="D75" t="n">
-        <v>0.875568</v>
+        <v>0.282286</v>
       </c>
       <c r="E75" t="n">
-        <v>-0.319582</v>
+        <v>-0.583039</v>
       </c>
       <c r="F75" t="n">
-        <v>0.462147</v>
+        <v>-0.5789029999999999</v>
       </c>
       <c r="G75" t="n">
-        <v>-0.07702199999999999</v>
+        <v>0.268523</v>
       </c>
       <c r="H75" t="n">
-        <v>0.89249</v>
+        <v>-0.585829</v>
       </c>
       <c r="I75" t="n">
-        <v>0.245303</v>
+        <v>-0.191234</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Die Hard: With a Vengeance (1995)</t>
+          <t>Lion King, The (1994)</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>-0.005185579913785093</v>
+        <v>6</v>
       </c>
       <c r="D76" t="n">
-        <v>0.692124</v>
+        <v>0.457468</v>
       </c>
       <c r="E76" t="n">
-        <v>0.406031</v>
+        <v>-0.236262</v>
       </c>
       <c r="F76" t="n">
-        <v>-0.689604</v>
+        <v>-0.719371</v>
       </c>
       <c r="G76" t="n">
-        <v>1.048333</v>
+        <v>0.279277</v>
       </c>
       <c r="H76" t="n">
-        <v>-0.08913699999999999</v>
+        <v>0.480993</v>
       </c>
       <c r="I76" t="n">
-        <v>-0.28635</v>
+        <v>-0.588977</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Meet the Parents (2000)</t>
+          <t>Sin City (2005)</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>-0.000518335890903191</v>
+        <v>9</v>
       </c>
       <c r="D77" t="n">
-        <v>0.234633</v>
+        <v>-1.174844</v>
       </c>
       <c r="E77" t="n">
-        <v>-0.364501</v>
+        <v>1.34822</v>
       </c>
       <c r="F77" t="n">
-        <v>-0.705371</v>
+        <v>0.570489</v>
       </c>
       <c r="G77" t="n">
-        <v>-0.069191</v>
+        <v>0.283971</v>
       </c>
       <c r="H77" t="n">
-        <v>-0.561307</v>
+        <v>-0.42946</v>
       </c>
       <c r="I77" t="n">
-        <v>-0.221236</v>
+        <v>-0.974198</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Speed (1994)</t>
+          <t>Beauty and the Beast (1991)</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>-0.004107877545169244</v>
+        <v>2</v>
       </c>
       <c r="D78" t="n">
-        <v>0.135632</v>
+        <v>0.438021</v>
       </c>
       <c r="E78" t="n">
-        <v>-0.647521</v>
+        <v>-1.024345</v>
       </c>
       <c r="F78" t="n">
-        <v>-1.55715</v>
+        <v>-0.626513</v>
       </c>
       <c r="G78" t="n">
-        <v>0.094816</v>
+        <v>0.288004</v>
       </c>
       <c r="H78" t="n">
-        <v>-0.480833</v>
+        <v>-0.133778</v>
       </c>
       <c r="I78" t="n">
-        <v>0.658863</v>
+        <v>-1.079223</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Star Wars: Episode V - The Empire Strikes Back (1980)</t>
+          <t>Back to the Future (1985)</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>-0.009958961489089395</v>
+        <v>4</v>
       </c>
       <c r="D79" t="n">
-        <v>-0.647379</v>
+        <v>0.257897</v>
       </c>
       <c r="E79" t="n">
-        <v>-0.566604</v>
+        <v>-0.661257</v>
       </c>
       <c r="F79" t="n">
-        <v>0.349584</v>
+        <v>-0.162848</v>
       </c>
       <c r="G79" t="n">
-        <v>0.082728</v>
+        <v>0.291349</v>
       </c>
       <c r="H79" t="n">
-        <v>1.256632</v>
+        <v>0.482955</v>
       </c>
       <c r="I79" t="n">
-        <v>-0.747074</v>
+        <v>-0.058067</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Star Wars: Episode VI - Return of the Jedi (1983)</t>
+          <t>Dark Knight, The (2008)</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.005913803624674758</v>
+        <v>3</v>
       </c>
       <c r="D80" t="n">
-        <v>-0.612156</v>
+        <v>-0.362395</v>
       </c>
       <c r="E80" t="n">
-        <v>-0.8104170000000001</v>
+        <v>0.441177</v>
       </c>
       <c r="F80" t="n">
-        <v>-0.067179</v>
+        <v>0.460574</v>
       </c>
       <c r="G80" t="n">
-        <v>0.222448</v>
+        <v>0.296781</v>
       </c>
       <c r="H80" t="n">
-        <v>1.080815</v>
+        <v>0.745397</v>
       </c>
       <c r="I80" t="n">
-        <v>-0.738045</v>
+        <v>0.9879520000000001</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Star Wars: Episode II - Attack of the Clones (2002)</t>
+          <t>Batman Forever (1995)</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>-0.07118385892739264</v>
+        <v>3</v>
       </c>
       <c r="D81" t="n">
-        <v>1.052404</v>
+        <v>0.087715</v>
       </c>
       <c r="E81" t="n">
-        <v>0.753224</v>
+        <v>0.004544</v>
       </c>
       <c r="F81" t="n">
-        <v>-1.531839</v>
+        <v>-1.690647</v>
       </c>
       <c r="G81" t="n">
-        <v>0.09943</v>
+        <v>0.301528</v>
       </c>
       <c r="H81" t="n">
-        <v>-0.746401</v>
+        <v>-1.182924</v>
       </c>
       <c r="I81" t="n">
-        <v>-0.7899</v>
+        <v>-0.403095</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Traffic (2000)</t>
+          <t>Mission: Impossible II (2000)</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>-0.01079437714200836</v>
+        <v>5</v>
       </c>
       <c r="D82" t="n">
-        <v>0.63268</v>
+        <v>0.538805</v>
       </c>
       <c r="E82" t="n">
-        <v>-0.558137</v>
+        <v>-0.211818</v>
       </c>
       <c r="F82" t="n">
-        <v>0.472564</v>
+        <v>-1.755887</v>
       </c>
       <c r="G82" t="n">
-        <v>0.322355</v>
+        <v>0.310784</v>
       </c>
       <c r="H82" t="n">
-        <v>0.607359</v>
+        <v>-1.39709</v>
       </c>
       <c r="I82" t="n">
-        <v>0.330394</v>
+        <v>-0.56005</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Patriot, The (2000)</t>
+          <t>Traffic (2000)</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>-0.004599316302700262</v>
+        <v>5</v>
       </c>
       <c r="D83" t="n">
-        <v>0.804366</v>
+        <v>0.63268</v>
       </c>
       <c r="E83" t="n">
-        <v>-0.246102</v>
+        <v>-0.558137</v>
       </c>
       <c r="F83" t="n">
-        <v>-1.203248</v>
+        <v>0.472564</v>
       </c>
       <c r="G83" t="n">
-        <v>-0.282312</v>
+        <v>0.322355</v>
       </c>
       <c r="H83" t="n">
-        <v>-0.291594</v>
+        <v>0.607359</v>
       </c>
       <c r="I83" t="n">
-        <v>-0.234564</v>
+        <v>0.330394</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>83</v>
+        <v>5</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Stargate (1994)</t>
+          <t>Pirates of the Caribbean: The Curse of the Black Pearl (2003)</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>-0.0001831388185485682</v>
+        <v>1</v>
       </c>
       <c r="D84" t="n">
-        <v>-0.042177</v>
+        <v>0.192967</v>
       </c>
       <c r="E84" t="n">
-        <v>-0.205697</v>
+        <v>0.262919</v>
       </c>
       <c r="F84" t="n">
-        <v>-0.47166</v>
+        <v>-0.116306</v>
       </c>
       <c r="G84" t="n">
-        <v>0.456668</v>
+        <v>0.322482</v>
       </c>
       <c r="H84" t="n">
-        <v>-0.364988</v>
+        <v>0.723021</v>
       </c>
       <c r="I84" t="n">
-        <v>-0.268515</v>
+        <v>-0.82364</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Bourne Identity, The (2002)</t>
+          <t>Erin Brockovich (2000)</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>-4.253517520129322e-05</v>
+        <v>9</v>
       </c>
       <c r="D85" t="n">
-        <v>0.266225</v>
+        <v>1.581845</v>
       </c>
       <c r="E85" t="n">
-        <v>0.500795</v>
+        <v>-0.62645</v>
       </c>
       <c r="F85" t="n">
-        <v>-0.162073</v>
+        <v>-0.213707</v>
       </c>
       <c r="G85" t="n">
-        <v>-0.345967</v>
+        <v>0.343191</v>
       </c>
       <c r="H85" t="n">
-        <v>0.059598</v>
+        <v>-0.639564</v>
       </c>
       <c r="I85" t="n">
-        <v>-0.095469</v>
+        <v>-0.133499</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Bourne Supremacy, The (2004)</t>
+          <t>Almost Famous (2000)</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>-0.002444897749739449</v>
+        <v>5</v>
       </c>
       <c r="D86" t="n">
-        <v>0.212682</v>
+        <v>0.618167</v>
       </c>
       <c r="E86" t="n">
-        <v>0.284779</v>
+        <v>0.041198</v>
       </c>
       <c r="F86" t="n">
-        <v>-0.921839</v>
+        <v>-0.129813</v>
       </c>
       <c r="G86" t="n">
-        <v>-1.301435</v>
+        <v>0.388409</v>
       </c>
       <c r="H86" t="n">
-        <v>0.223149</v>
+        <v>0.182649</v>
       </c>
       <c r="I86" t="n">
-        <v>-0.150782</v>
+        <v>0.379338</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Ace Ventura: Pet Detective (1994)</t>
+          <t>Unbreakable (2000)</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>-0.0003650133451154303</v>
+        <v>5</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.00572</v>
+        <v>-0.74914</v>
       </c>
       <c r="E87" t="n">
-        <v>-0.077822</v>
+        <v>0.319645</v>
       </c>
       <c r="F87" t="n">
-        <v>-1.025428</v>
+        <v>-0.141918</v>
       </c>
       <c r="G87" t="n">
-        <v>1.623392</v>
+        <v>0.41697</v>
       </c>
       <c r="H87" t="n">
-        <v>-1.117656</v>
+        <v>-0.713696</v>
       </c>
       <c r="I87" t="n">
-        <v>-0.440731</v>
+        <v>-0.78928</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>87</v>
+        <v>13</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Charlie's Angels (2000)</t>
+          <t>Snatch (2000)</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.1043542310852992</v>
+        <v>8</v>
       </c>
       <c r="D88" t="n">
-        <v>0.665559</v>
+        <v>0.62363</v>
       </c>
       <c r="E88" t="n">
-        <v>-0.472255</v>
+        <v>0.194445</v>
       </c>
       <c r="F88" t="n">
-        <v>-1.249498</v>
+        <v>0.449922</v>
       </c>
       <c r="G88" t="n">
-        <v>0.18608</v>
+        <v>0.439904</v>
       </c>
       <c r="H88" t="n">
-        <v>-1.503001</v>
+        <v>-0.059525</v>
       </c>
       <c r="I88" t="n">
-        <v>-0.950063</v>
+        <v>-0.250803</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Fugitive, The (1993)</t>
+          <t>Kill Bill: Vol, 2 (2004)</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.0007678155381266499</v>
+        <v>1</v>
       </c>
       <c r="D89" t="n">
-        <v>0.399062</v>
+        <v>0.68703</v>
       </c>
       <c r="E89" t="n">
-        <v>-0.6332140000000001</v>
+        <v>0.073925</v>
       </c>
       <c r="F89" t="n">
-        <v>-0.5366030000000001</v>
+        <v>1.732061</v>
       </c>
       <c r="G89" t="n">
-        <v>0.065729</v>
+        <v>0.449929</v>
       </c>
       <c r="H89" t="n">
-        <v>0.158757</v>
+        <v>-0.18962</v>
       </c>
       <c r="I89" t="n">
-        <v>0.542654</v>
+        <v>-1.638298</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Chicken Run (2000)</t>
+          <t>Donnie Darko (2001)</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>-0.005466528231231537</v>
+        <v>9</v>
       </c>
       <c r="D90" t="n">
-        <v>0.089708</v>
+        <v>0.517054</v>
       </c>
       <c r="E90" t="n">
-        <v>-1.196121</v>
+        <v>-0.171271</v>
       </c>
       <c r="F90" t="n">
-        <v>-0.289824</v>
+        <v>0.892353</v>
       </c>
       <c r="G90" t="n">
-        <v>-0.499809</v>
+        <v>0.456009</v>
       </c>
       <c r="H90" t="n">
-        <v>-0.83693</v>
+        <v>-0.563917</v>
       </c>
       <c r="I90" t="n">
-        <v>-0.420221</v>
+        <v>-0.297528</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Cast Away (2000)</t>
+          <t>Stargate (1994)</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>-0.04183527198646862</v>
+        <v>1</v>
       </c>
       <c r="D91" t="n">
-        <v>1.014575</v>
+        <v>-0.042177</v>
       </c>
       <c r="E91" t="n">
-        <v>0.403793</v>
+        <v>-0.205697</v>
       </c>
       <c r="F91" t="n">
-        <v>-0.477961</v>
+        <v>-0.47166</v>
       </c>
       <c r="G91" t="n">
-        <v>-0.450861</v>
+        <v>0.456668</v>
       </c>
       <c r="H91" t="n">
-        <v>0.355866</v>
+        <v>-0.364988</v>
       </c>
       <c r="I91" t="n">
-        <v>-1.331613</v>
+        <v>-0.268515</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Dumb &amp; Dumber (Dumb and Dumber) (1994)</t>
+          <t>True Lies (1994)</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.01035368211016306</v>
+        <v>9</v>
       </c>
       <c r="D92" t="n">
-        <v>0.488822</v>
+        <v>0.266676</v>
       </c>
       <c r="E92" t="n">
-        <v>-0.161945</v>
+        <v>-0.679851</v>
       </c>
       <c r="F92" t="n">
-        <v>-1.203414</v>
+        <v>-1.040011</v>
       </c>
       <c r="G92" t="n">
-        <v>1.852664</v>
+        <v>0.502973</v>
       </c>
       <c r="H92" t="n">
-        <v>-0.305408</v>
+        <v>-0.280113</v>
       </c>
       <c r="I92" t="n">
-        <v>-0.192081</v>
+        <v>-0.063542</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Lion King, The (1994)</t>
+          <t>Harry Potter and the Sorcerer's Stone (a,k,a, Harry Potter and the Philosopher's Stone) (2001)</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>-0.00615148238685488</v>
+        <v>6</v>
       </c>
       <c r="D93" t="n">
-        <v>0.457468</v>
+        <v>1.359601</v>
       </c>
       <c r="E93" t="n">
-        <v>-0.236262</v>
+        <v>0.07443900000000001</v>
       </c>
       <c r="F93" t="n">
-        <v>-0.719371</v>
+        <v>-0.668836</v>
       </c>
       <c r="G93" t="n">
-        <v>0.279277</v>
+        <v>0.532676</v>
       </c>
       <c r="H93" t="n">
-        <v>0.480993</v>
+        <v>-0.447798</v>
       </c>
       <c r="I93" t="n">
-        <v>-0.588977</v>
+        <v>-0.197322</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Clear and Present Danger (1994)</t>
+          <t>Batman (1989)</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>7.374917115419967e-05</v>
+        <v>8</v>
       </c>
       <c r="D94" t="n">
-        <v>0.521285</v>
+        <v>0.524029</v>
       </c>
       <c r="E94" t="n">
-        <v>-0.234548</v>
+        <v>-0.148073</v>
       </c>
       <c r="F94" t="n">
-        <v>-0.772875</v>
+        <v>0.013642</v>
       </c>
       <c r="G94" t="n">
-        <v>0.154113</v>
+        <v>0.54508</v>
       </c>
       <c r="H94" t="n">
-        <v>-0.073448</v>
+        <v>-0.6282489999999999</v>
       </c>
       <c r="I94" t="n">
-        <v>-0.068948</v>
+        <v>-0.432091</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Unbreakable (2000)</t>
+          <t>Terminator 2: Judgment Day (1991)</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.007982107175148126</v>
+        <v>4</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.74914</v>
+        <v>0.027123</v>
       </c>
       <c r="E95" t="n">
-        <v>0.319645</v>
+        <v>-0.178035</v>
       </c>
       <c r="F95" t="n">
-        <v>-0.141918</v>
+        <v>-0.365473</v>
       </c>
       <c r="G95" t="n">
-        <v>0.41697</v>
+        <v>0.552849</v>
       </c>
       <c r="H95" t="n">
-        <v>-0.713696</v>
+        <v>0.199415</v>
       </c>
       <c r="I95" t="n">
-        <v>-0.78928</v>
+        <v>0.163796</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Rock, The (1996)</t>
+          <t>Mask, The (1994)</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>-0.000711927147657295</v>
+        <v>7</v>
       </c>
       <c r="D96" t="n">
-        <v>0.139304</v>
+        <v>0.43985</v>
       </c>
       <c r="E96" t="n">
-        <v>-0.48713</v>
+        <v>-0.116494</v>
       </c>
       <c r="F96" t="n">
-        <v>-0.7407049999999999</v>
+        <v>-1.091039</v>
       </c>
       <c r="G96" t="n">
-        <v>-0.303868</v>
+        <v>0.636489</v>
       </c>
       <c r="H96" t="n">
-        <v>-0.449029</v>
+        <v>-0.856053</v>
       </c>
       <c r="I96" t="n">
-        <v>-0.103806</v>
+        <v>-0.431378</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>96</v>
+        <v>50</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Incredibles, The (2004)</t>
+          <t>Independence Day (a,k,a, ID4) (1996)</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0.04620101684431009</v>
+        <v>5</v>
       </c>
       <c r="D97" t="n">
-        <v>0.49024</v>
+        <v>0.385232</v>
       </c>
       <c r="E97" t="n">
-        <v>-0.924104</v>
+        <v>-0.440648</v>
       </c>
       <c r="F97" t="n">
-        <v>0.69907</v>
+        <v>-1.013302</v>
       </c>
       <c r="G97" t="n">
-        <v>-1.499481</v>
+        <v>0.733044</v>
       </c>
       <c r="H97" t="n">
-        <v>-0.09470099999999999</v>
+        <v>-0.587827</v>
       </c>
       <c r="I97" t="n">
-        <v>-1.02732</v>
+        <v>-0.979442</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Beauty and the Beast (1991)</t>
+          <t>Fight Club (1999)</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.01168868572762691</v>
+        <v>7</v>
       </c>
       <c r="D98" t="n">
-        <v>0.438021</v>
+        <v>-0.289515</v>
       </c>
       <c r="E98" t="n">
-        <v>-1.024345</v>
+        <v>0.565428</v>
       </c>
       <c r="F98" t="n">
-        <v>-0.626513</v>
+        <v>1.511413</v>
       </c>
       <c r="G98" t="n">
-        <v>0.288004</v>
+        <v>0.8930399999999999</v>
       </c>
       <c r="H98" t="n">
-        <v>-0.133778</v>
+        <v>0.252663</v>
       </c>
       <c r="I98" t="n">
-        <v>-1.079223</v>
+        <v>0.729976</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>X-Men (2000)</t>
+          <t>Die Hard: With a Vengeance (1995)</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>-8.283778732466473e-05</v>
+        <v>2</v>
       </c>
       <c r="D99" t="n">
-        <v>0.471031</v>
+        <v>0.692124</v>
       </c>
       <c r="E99" t="n">
-        <v>-0.20257</v>
+        <v>0.406031</v>
       </c>
       <c r="F99" t="n">
-        <v>-0.10811</v>
+        <v>-0.689604</v>
       </c>
       <c r="G99" t="n">
-        <v>-0.02124</v>
+        <v>1.048333</v>
       </c>
       <c r="H99" t="n">
-        <v>-0.8985</v>
+        <v>-0.08913699999999999</v>
       </c>
       <c r="I99" t="n">
-        <v>-0.42079</v>
+        <v>-0.28635</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>X2: X-Men United (2003)</t>
+          <t>Ace Ventura: Pet Detective (1994)</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0.00447109383149635</v>
+        <v>4</v>
       </c>
       <c r="D100" t="n">
-        <v>0.943534</v>
+        <v>-0.00572</v>
       </c>
       <c r="E100" t="n">
-        <v>0.084534</v>
+        <v>-0.077822</v>
       </c>
       <c r="F100" t="n">
-        <v>-0.235003</v>
+        <v>-1.025428</v>
       </c>
       <c r="G100" t="n">
-        <v>-0.665734</v>
+        <v>1.623392</v>
       </c>
       <c r="H100" t="n">
-        <v>-0.94687</v>
+        <v>-1.117656</v>
       </c>
       <c r="I100" t="n">
-        <v>-0.378408</v>
+        <v>-0.440731</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>True Lies (1994)</t>
+          <t>Dumb &amp; Dumber (Dumb and Dumber) (1994)</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.001688007699511539</v>
+        <v>8</v>
       </c>
       <c r="D101" t="n">
-        <v>0.266676</v>
+        <v>0.488822</v>
       </c>
       <c r="E101" t="n">
-        <v>-0.679851</v>
+        <v>-0.161945</v>
       </c>
       <c r="F101" t="n">
-        <v>-1.040011</v>
+        <v>-1.203414</v>
       </c>
       <c r="G101" t="n">
-        <v>0.502973</v>
+        <v>1.852664</v>
       </c>
       <c r="H101" t="n">
-        <v>-0.280113</v>
+        <v>-0.305408</v>
       </c>
       <c r="I101" t="n">
-        <v>-0.063542</v>
+        <v>-0.192081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>